<commit_message>
Modbus Register E3DC Import Datei
</commit_message>
<xml_diff>
--- a/Modbus_E3DC_Import.xlsx
+++ b/Modbus_E3DC_Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.60\RaspberryMatic\ioBroker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\E3DC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{234C836A-C7F8-4E9E-881A-6DE6A7C527B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845B6BD1-65FB-4FC7-946F-7C15C4909414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-600" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modbus_E3DC" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="153">
   <si>
     <t>_address</t>
   </si>
@@ -493,6 +493,9 @@
   </si>
   <si>
     <t>SG Ready-Status</t>
+  </si>
+  <si>
+    <t>0.01</t>
   </si>
 </sst>
 </file>
@@ -528,9 +531,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -886,7 +892,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C775C727-74CE-4A5C-B0EE-80DC24CA41B0}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2429,8 +2437,8 @@
       <c r="F33">
         <v>1</v>
       </c>
-      <c r="G33">
-        <v>1</v>
+      <c r="G33" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -2476,8 +2484,8 @@
       <c r="F34">
         <v>1</v>
       </c>
-      <c r="G34">
-        <v>1</v>
+      <c r="G34" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2523,8 +2531,8 @@
       <c r="F35">
         <v>1</v>
       </c>
-      <c r="G35">
-        <v>1</v>
+      <c r="G35" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="H35">
         <v>0</v>

</xml_diff>